<commit_message>
them chuc nang lay du lieu log json
</commit_message>
<xml_diff>
--- a/Source/temp.xlsx
+++ b/Source/temp.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="55">
   <si>
     <t>Title</t>
   </si>
@@ -29,19 +29,16 @@
     <t>..\log\GGB1UD22209318EE__wifi_cal_231909_PASS.txt</t>
   </si>
   <si>
-    <t>38.TEST_VERIFY EVM POWER MASK 2412 MCS0 VHT BW-20 ANT2 | EVM_DB_AVG_S1</t>
+    <t>38.TEST_VERIFY EVM POWER MASK 2412 MCS0 VHT BW-20 ANT2</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t xml:space="preserve"> dB</t>
-  </si>
-  <si>
-    <t>38.TEST_VERIFY EVM POWER MASK 2412 MCS0 VHT BW-20 ANT2 | POWER_AVG_DBM</t>
-  </si>
-  <si>
-    <t>46.TEST_VERIFY EVM POWER MASK 2437 MCS11 HE_SU BW-40 ANT2 | EVM_DB_AVG_S1</t>
+    <t xml:space="preserve"> s</t>
+  </si>
+  <si>
+    <t>46.TEST_VERIFY EVM POWER MASK 2437 MCS11 HE_SU BW-40 ANT2</t>
   </si>
   <si>
     <t>..\log\GGB1UD222093194C__wifi_cal_230844_PASS.txt</t>
@@ -224,7 +221,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:C51"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -240,22 +237,16 @@
       <c r="C1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="n">
-        <v>-5.0</v>
-      </c>
-      <c r="C2" t="n">
-        <v>25.25</v>
-      </c>
-      <c r="D2" t="n">
-        <v>-35.0</v>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3">
@@ -265,10 +256,7 @@
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="n">
-        <v>22.75</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="C3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -282,666 +270,522 @@
       <c r="C4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>-15.99</v>
+        <v>0.763</v>
       </c>
       <c r="C5" t="n">
-        <v>24.44</v>
-      </c>
-      <c r="D5" t="n">
-        <v>-42.89</v>
+        <v>1.368</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" t="n">
-        <v>-15.83</v>
+        <v>0.752</v>
       </c>
       <c r="C6" t="n">
-        <v>24.54</v>
-      </c>
-      <c r="D6" t="n">
-        <v>-41.99</v>
+        <v>0.864</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" t="n">
-        <v>-15.78</v>
+        <v>1.319</v>
       </c>
       <c r="C7" t="n">
-        <v>24.41</v>
-      </c>
-      <c r="D7" t="n">
-        <v>-43.45</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" t="n">
-        <v>-16.02</v>
+        <v>1.467</v>
       </c>
       <c r="C8" t="n">
-        <v>24.54</v>
-      </c>
-      <c r="D8" t="n">
-        <v>-42.4</v>
+        <v>1.039</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" t="n">
-        <v>-16.18</v>
+        <v>0.754</v>
       </c>
       <c r="C9" t="n">
-        <v>24.36</v>
-      </c>
-      <c r="D9" t="n">
-        <v>-42.66</v>
+        <v>2.335</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" t="n">
-        <v>-16.21</v>
+        <v>0.82</v>
       </c>
       <c r="C10" t="n">
-        <v>24.52</v>
-      </c>
-      <c r="D10" t="n">
-        <v>-42.54</v>
+        <v>0.892</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" t="n">
-        <v>-16.34</v>
+        <v>1.523</v>
       </c>
       <c r="C11" t="n">
-        <v>24.53</v>
-      </c>
-      <c r="D11" t="n">
-        <v>-42.75</v>
+        <v>0.942</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" t="n">
-        <v>-16.0</v>
+        <v>0.773</v>
       </c>
       <c r="C12" t="n">
-        <v>24.51</v>
-      </c>
-      <c r="D12" t="n">
-        <v>-40.17</v>
+        <v>1.322</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13" t="n">
-        <v>-15.97</v>
+        <v>0.972</v>
       </c>
       <c r="C13" t="n">
-        <v>24.52</v>
-      </c>
-      <c r="D13" t="n">
-        <v>-42.28</v>
+        <v>0.977</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14" t="n">
-        <v>-15.99</v>
+        <v>0.742</v>
       </c>
       <c r="C14" t="n">
-        <v>24.47</v>
-      </c>
-      <c r="D14" t="n">
-        <v>-42.91</v>
+        <v>0.889</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15" t="n">
-        <v>-16.02</v>
+        <v>0.777</v>
       </c>
       <c r="C15" t="n">
-        <v>24.28</v>
-      </c>
-      <c r="D15" t="n">
-        <v>-42.29</v>
+        <v>0.956</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B16" t="n">
-        <v>-15.98</v>
+        <v>0.742</v>
       </c>
       <c r="C16" t="n">
-        <v>24.46</v>
-      </c>
-      <c r="D16" t="n">
-        <v>-43.32</v>
+        <v>0.93</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B17" t="n">
-        <v>-16.17</v>
+        <v>1.01</v>
       </c>
       <c r="C17" t="n">
-        <v>24.53</v>
-      </c>
-      <c r="D17" t="n">
-        <v>-43.57</v>
+        <v>1.275</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18" t="n">
-        <v>-15.92</v>
+        <v>0.89</v>
       </c>
       <c r="C18" t="n">
-        <v>24.55</v>
-      </c>
-      <c r="D18" t="n">
-        <v>-42.23</v>
+        <v>1.543</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B19" t="n">
-        <v>-15.92</v>
+        <v>0.757</v>
       </c>
       <c r="C19" t="n">
-        <v>24.6</v>
-      </c>
-      <c r="D19" t="n">
-        <v>-42.0</v>
+        <v>0.941</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B20" t="n">
-        <v>-16.17</v>
+        <v>0.759</v>
       </c>
       <c r="C20" t="n">
-        <v>24.52</v>
-      </c>
-      <c r="D20" t="n">
-        <v>-41.76</v>
+        <v>0.879</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B21" t="n">
-        <v>-16.17</v>
+        <v>0.779</v>
       </c>
       <c r="C21" t="n">
-        <v>24.37</v>
-      </c>
-      <c r="D21" t="n">
-        <v>-42.36</v>
+        <v>0.899</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B22" t="n">
-        <v>-15.72</v>
+        <v>0.735</v>
       </c>
       <c r="C22" t="n">
-        <v>24.44</v>
-      </c>
-      <c r="D22" t="n">
-        <v>-40.69</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B23" t="n">
-        <v>-15.95</v>
+        <v>0.785</v>
       </c>
       <c r="C23" t="n">
-        <v>24.61</v>
-      </c>
-      <c r="D23" t="n">
-        <v>-42.25</v>
+        <v>0.884</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B24" t="n">
-        <v>-15.95</v>
+        <v>0.742</v>
       </c>
       <c r="C24" t="n">
-        <v>24.53</v>
-      </c>
-      <c r="D24" t="n">
-        <v>-42.79</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B25" t="n">
-        <v>-16.08</v>
+        <v>1.504</v>
       </c>
       <c r="C25" t="n">
-        <v>24.61</v>
-      </c>
-      <c r="D25" t="n">
-        <v>-42.47</v>
+        <v>1.544</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B26" t="n">
-        <v>-16.21</v>
+        <v>0.781</v>
       </c>
       <c r="C26" t="n">
-        <v>24.56</v>
-      </c>
-      <c r="D26" t="n">
-        <v>-42.41</v>
+        <v>1.482</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B27" t="n">
-        <v>-16.14</v>
+        <v>1.504</v>
       </c>
       <c r="C27" t="n">
-        <v>24.59</v>
-      </c>
-      <c r="D27" t="n">
-        <v>-42.57</v>
+        <v>0.943</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B28" t="n">
-        <v>-15.52</v>
+        <v>0.845</v>
       </c>
       <c r="C28" t="n">
-        <v>24.64</v>
-      </c>
-      <c r="D28" t="n">
-        <v>-41.32</v>
+        <v>1.103</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B29" t="n">
-        <v>-15.96</v>
+        <v>0.815</v>
       </c>
       <c r="C29" t="n">
-        <v>24.55</v>
-      </c>
-      <c r="D29" t="n">
-        <v>-42.18</v>
+        <v>0.933</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B30" t="n">
-        <v>-15.81</v>
+        <v>0.781</v>
       </c>
       <c r="C30" t="n">
-        <v>24.48</v>
-      </c>
-      <c r="D30" t="n">
-        <v>-40.85</v>
+        <v>0.881</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B31" t="n">
-        <v>-16.11</v>
+        <v>0.854</v>
       </c>
       <c r="C31" t="n">
-        <v>24.37</v>
-      </c>
-      <c r="D31" t="n">
-        <v>-43.27</v>
+        <v>0.903</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B32" t="n">
-        <v>-15.97</v>
+        <v>0.754</v>
       </c>
       <c r="C32" t="n">
-        <v>24.55</v>
-      </c>
-      <c r="D32" t="n">
-        <v>-41.96</v>
+        <v>1.398</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B33" t="n">
-        <v>-16.2</v>
+        <v>0.771</v>
       </c>
       <c r="C33" t="n">
-        <v>24.51</v>
-      </c>
-      <c r="D33" t="n">
-        <v>-41.47</v>
+        <v>1.623</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B34" t="n">
-        <v>-16.13</v>
+        <v>0.821</v>
       </c>
       <c r="C34" t="n">
-        <v>24.42</v>
-      </c>
-      <c r="D34" t="n">
-        <v>-42.92</v>
+        <v>1.322</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B35" t="n">
-        <v>-15.98</v>
+        <v>0.782</v>
       </c>
       <c r="C35" t="n">
-        <v>24.53</v>
-      </c>
-      <c r="D35" t="n">
-        <v>-41.8</v>
+        <v>0.894</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B36" t="n">
-        <v>-16.14</v>
+        <v>0.806</v>
       </c>
       <c r="C36" t="n">
-        <v>24.52</v>
-      </c>
-      <c r="D36" t="n">
-        <v>-42.88</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B37" t="n">
-        <v>-16.08</v>
+        <v>0.761</v>
       </c>
       <c r="C37" t="n">
-        <v>24.4</v>
-      </c>
-      <c r="D37" t="n">
-        <v>-42.0</v>
+        <v>0.864</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B38" t="n">
-        <v>-15.81</v>
+        <v>1.361</v>
       </c>
       <c r="C38" t="n">
-        <v>24.69</v>
-      </c>
-      <c r="D38" t="n">
-        <v>-42.55</v>
+        <v>0.929</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B39" t="n">
-        <v>-16.13</v>
+        <v>0.815</v>
       </c>
       <c r="C39" t="n">
-        <v>24.3</v>
-      </c>
-      <c r="D39" t="n">
-        <v>-42.76</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B40" t="n">
-        <v>-16.11</v>
+        <v>0.759</v>
       </c>
       <c r="C40" t="n">
-        <v>24.48</v>
-      </c>
-      <c r="D40" t="n">
-        <v>-43.25</v>
+        <v>0.913</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B41" t="n">
-        <v>-16.01</v>
+        <v>1.564</v>
       </c>
       <c r="C41" t="n">
-        <v>24.37</v>
-      </c>
-      <c r="D41" t="n">
-        <v>-42.9</v>
+        <v>1.632</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B42" t="n">
-        <v>-16.34</v>
+        <v>0.824</v>
       </c>
       <c r="C42" t="n">
-        <v>24.33</v>
-      </c>
-      <c r="D42" t="n">
-        <v>-39.95</v>
+        <v>0.886</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B43" t="n">
-        <v>-16.13</v>
+        <v>0.823</v>
       </c>
       <c r="C43" t="n">
-        <v>24.53</v>
-      </c>
-      <c r="D43" t="n">
-        <v>-43.39</v>
+        <v>1.053</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B44" t="n">
-        <v>-16.19</v>
+        <v>1.238</v>
       </c>
       <c r="C44" t="n">
-        <v>24.3</v>
-      </c>
-      <c r="D44" t="n">
-        <v>-39.23</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B45" t="n">
-        <v>-16.09</v>
+        <v>1.569</v>
       </c>
       <c r="C45" t="n">
-        <v>24.53</v>
-      </c>
-      <c r="D45" t="n">
-        <v>-43.02</v>
+        <v>0.895</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B46" t="n">
-        <v>-16.16</v>
+        <v>0.785</v>
       </c>
       <c r="C46" t="n">
-        <v>24.42</v>
-      </c>
-      <c r="D46" t="n">
-        <v>-42.13</v>
+        <v>0.869</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B47" t="n">
-        <v>-16.33</v>
+        <v>0.824</v>
       </c>
       <c r="C47" t="n">
-        <v>24.53</v>
-      </c>
-      <c r="D47" t="n">
-        <v>-41.09</v>
+        <v>1.418</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B48" t="n">
-        <v>-15.86</v>
+        <v>1.308</v>
       </c>
       <c r="C48" t="n">
-        <v>24.41</v>
-      </c>
-      <c r="D48" t="n">
-        <v>-41.39</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B49" t="n">
-        <v>-16.15</v>
+        <v>0.736</v>
       </c>
       <c r="C49" t="n">
-        <v>24.52</v>
-      </c>
-      <c r="D49" t="n">
-        <v>-43.55</v>
+        <v>0.959</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B50" t="n">
-        <v>-16.04</v>
+        <v>0.763</v>
       </c>
       <c r="C50" t="n">
-        <v>24.54</v>
-      </c>
-      <c r="D50" t="n">
-        <v>-43.47</v>
+        <v>1.547</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B51" t="n">
-        <v>-16.21</v>
+        <v>0.773</v>
       </c>
       <c r="C51" t="n">
-        <v>24.54</v>
-      </c>
-      <c r="D51" t="n">
-        <v>-43.47</v>
+        <v>0.921</v>
       </c>
     </row>
   </sheetData>

</xml_diff>